<commit_message>
terminada cache, inicio relatório
</commit_message>
<xml_diff>
--- a/graficos.xlsx
+++ b/graficos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivis\Documents\GitHub\AOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaceFaculdade\QuartoSemestre\AOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F23CE7DD-E924-4ADA-923B-FBF7DEE9C33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB02E28F-300F-4B30-955E-5A483E643EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{74572744-394E-4295-AEB7-9920350B769E}"/>
   </bookViews>
@@ -220,6 +220,9 @@
                 <c:pt idx="1">
                   <c:v>9660</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>10100</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -292,10 +295,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2019.8</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8880</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -369,10 +375,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11277.7</c:v>
+                  <c:v>11278</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>29020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29940</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -451,6 +460,9 @@
                 <c:pt idx="1">
                   <c:v>11912.9</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>12480</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -527,6 +539,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>28200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1780,7 +1795,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1817,10 +1832,10 @@
         <v>2160</v>
       </c>
       <c r="C2" s="1">
-        <v>2019.8</v>
+        <v>2020</v>
       </c>
       <c r="D2" s="1">
-        <v>11277.7</v>
+        <v>11278</v>
       </c>
       <c r="E2" s="1">
         <v>5740</v>
@@ -1853,11 +1868,21 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="B4" s="1">
+        <v>10100</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9400</v>
+      </c>
+      <c r="D4" s="1">
+        <v>29940</v>
+      </c>
+      <c r="E4" s="1">
+        <v>12480</v>
+      </c>
+      <c r="F4" s="1">
+        <v>28703</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>